<commit_message>
worked on evaluatie gj2018
</commit_message>
<xml_diff>
--- a/input/history.xlsx
+++ b/input/history.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10123"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\D-CD\SSD\(b) CAP-EC\01 Kernactiviteiten\OP-Declaratie\2019\1. berekeningen\5.b GPtools python\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Wouter SD/GPtools/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B237F5-79C1-E04A-B0D7-ABF2C85047E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="4800" activeTab="1"/>
+    <workbookView xWindow="3260" yWindow="1580" windowWidth="20160" windowHeight="13460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="realisatie" sheetId="1" r:id="rId1"/>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -435,16 +436,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,7 +826,24 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="B20" s="5"/>
+      <c r="A20">
+        <v>2018</v>
+      </c>
+      <c r="B20">
+        <v>497455</v>
+      </c>
+      <c r="C20">
+        <v>9200</v>
+      </c>
+      <c r="D20">
+        <v>150000</v>
+      </c>
+      <c r="E20">
+        <v>2500</v>
+      </c>
+      <c r="F20">
+        <v>19500</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -833,27 +851,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">

</xml_diff>